<commit_message>
added 4 csv files to resources folder
</commit_message>
<xml_diff>
--- a/Resources/contacts.xlsx
+++ b/Resources/contacts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tberton/Desktop/nflx_data_2_Fall_22/01-Lesson-Plans/03-ETL/2/Activities/06-Par-Mini_ETL_Project/Solved/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahkollmann/Project_2/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA862834-D96C-9D43-87C0-A2A9BCCC1B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEB7614-578C-064E-84ED-E5EBBF169C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="980" windowWidth="28560" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="1003">
   <si>
     <t>contact_info</t>
   </si>
   <si>
     <t>Note: The contact information needs to be separated into the following columns: contact_id,  first name, last name,  and email.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
   </si>
   <si>
     <t>{"contact_id": 4661, "name": "Cecilia Velasco", "email": "cecilia.velasco@rodrigues.fr"}</t>
@@ -3069,7 +3066,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3090,9 +3087,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3130,9 +3127,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3165,26 +3162,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3217,26 +3197,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3410,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A1004"/>
+  <dimension ref="A1:A1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3423,7 +3386,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -3432,13 +3395,13 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -8434,11 +8397,6 @@
     <row r="1003" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1003" t="s">
         <v>1001</v>
-      </c>
-    </row>
-    <row r="1004" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1004" t="s">
-        <v>1002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>